<commit_message>
Updated EV profiles source with RAMP-mobility results
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/ProRes1/TIMES_Energy_HDAM.xlsx
+++ b/Inputs/JRC_EU_TIMES/ProRes1/TIMES_Energy_HDAM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10459618_polimi_it/Documents/Università/Tesi (OneDrive)/Article PROres1 coupling/JRC-EU-TIMES Data/PROres/PROres raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10459618_polimi_it/Documents/Università/Tesi (OneDrive)/Final Simulations Dispa-SET/JRC-EU-TIMES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37F7AB86-908B-464C-94D4-E4265531DC11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ABEF16E-2D5F-45C3-B13D-2F7375FC1749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{D6FEAF58-0983-43DE-BAE8-438A0A918365}"/>
+    <workbookView xWindow="2070" yWindow="1125" windowWidth="14670" windowHeight="8325" xr2:uid="{8A82DFC8-7322-47A8-BC1D-C7D7406DD571}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Unit - activity1  /  Period  /  Process Description1</t>
   </si>
@@ -85,6 +87,9 @@
   </si>
   <si>
     <t>IE</t>
+  </si>
+  <si>
+    <t>IS</t>
   </si>
   <si>
     <t>IT</t>
@@ -505,8 +510,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D5BBC70-B10D-4CEF-9842-7BADE0872766}">
-  <dimension ref="A1:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B720831-E670-4BDB-9C88-F40EA3E500B0}">
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -677,10 +682,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="1">
-        <v>110.53400000000001</v>
+        <v>30.571999999999999</v>
       </c>
       <c r="C17" s="1">
-        <v>45.942</v>
+        <v>32.65</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -688,10 +693,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>1.879</v>
+        <v>110.53400000000001</v>
       </c>
       <c r="C18" s="1">
-        <v>0.10100000000000001</v>
+        <v>45.942</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -699,10 +704,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>0.39200000000000002</v>
+        <v>1.879</v>
       </c>
       <c r="C19" s="1">
-        <v>0.11700000000000001</v>
+        <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -710,7 +715,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>12.19</v>
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.11700000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,7 +726,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>512.24300000000005</v>
+        <v>12.19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -726,10 +734,7 @@
         <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>5.65</v>
-      </c>
-      <c r="C22" s="1">
-        <v>15.728</v>
+        <v>512.24300000000005</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -737,10 +742,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>23.902000000000001</v>
+        <v>5.65</v>
       </c>
       <c r="C23" s="1">
-        <v>16.888000000000002</v>
+        <v>15.728</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -748,10 +753,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="1">
-        <v>69.156000000000006</v>
+        <v>23.902000000000001</v>
       </c>
       <c r="C24" s="1">
-        <v>0.71599999999999997</v>
+        <v>16.888000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -759,10 +764,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>117.11799999999999</v>
+        <v>69.156000000000006</v>
       </c>
       <c r="C25" s="1">
-        <v>40.527000000000001</v>
+        <v>0.71599999999999997</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -770,10 +775,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="1">
-        <v>14.019</v>
+        <v>117.11799999999999</v>
       </c>
       <c r="C26" s="1">
-        <v>14.467000000000001</v>
+        <v>40.527000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -781,10 +786,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="1">
-        <v>9.9890000000000008</v>
+        <v>14.019</v>
       </c>
       <c r="C27" s="1">
-        <v>4.1760000000000002</v>
+        <v>14.467000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -792,9 +797,20 @@
         <v>29</v>
       </c>
       <c r="B28" s="1">
+        <v>9.9890000000000008</v>
+      </c>
+      <c r="C28" s="1">
+        <v>4.1760000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1">
         <v>11.837</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C29" s="1">
         <v>7.907</v>
       </c>
     </row>
@@ -810,8 +826,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA58F2CACE833A4EAC3C2718D7553EBC" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="aec9d4db9f94a4e7a09eb83c0739bc84">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7880897e-52c6-4ffd-85c8-5c6950347fc0" xmlns:ns4="8c824e80-41b8-4a07-a4d9-9d9814734933" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f498252f696c0305676dba07191acd81" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA58F2CACE833A4EAC3C2718D7553EBC" ma:contentTypeVersion="13" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="bb63102ff0d9eda75d0b4de88b67103d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7880897e-52c6-4ffd-85c8-5c6950347fc0" xmlns:ns4="8c824e80-41b8-4a07-a4d9-9d9814734933" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d343f4382375feb5aaefc2a566ff9801" ns3:_="" ns4:_="">
     <xsd:import namespace="7880897e-52c6-4ffd-85c8-5c6950347fc0"/>
     <xsd:import namespace="8c824e80-41b8-4a07-a4d9-9d9814734933"/>
     <xsd:element name="properties">
@@ -831,6 +847,8 @@
                 <xsd:element ref="ns4:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceKeyPoints" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -916,6 +934,18 @@
     <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="19" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="20" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1034,7 +1064,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23C4A46E-05AB-4FF3-8C1E-6104EED14208}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06464369-584A-4B0C-8EC9-7650E2E43C78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -1053,7 +1083,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7B57D74-6054-4860-8F0D-96F9356258A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9178F004-9097-4541-B43C-7068A62C01AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
@@ -1061,7 +1091,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{240B1B85-1B5E-4BF4-804B-F13F0C10EB89}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45C26B61-B5FA-423D-8120-2C348C5975D0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>

</xml_diff>